<commit_message>
new tables_dave.xlsx data and added more ablauf.
</commit_message>
<xml_diff>
--- a/presentation/data/tables_dave.xlsx
+++ b/presentation/data/tables_dave.xlsx
@@ -126,7 +126,7 @@
     <t xml:space="preserve">['AccType', 'Severity', 'Pedestrian', 'Bicycle', 'Motorcycle', 'Temperature', 'RainDur']</t>
   </si>
   <si>
-    <t xml:space="preserve">['AccType', 'Temperature', 'RainDur']</t>
+    <t xml:space="preserve">['Severity', 'AccType', 'Bicycle']</t>
   </si>
 </sst>
 </file>
@@ -236,7 +236,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -245,6 +245,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -287,6 +291,10 @@
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -313,6 +321,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -320,303 +331,303 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="3"/>
+      <c r="B3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3" t="n">
+      <c r="B7" s="4" t="n">
         <v>0.764170986657602</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="5"/>
+      <c r="B8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="n">
+      <c r="B10" s="4" t="n">
         <v>0.317179</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="n">
+      <c r="B11" s="4" t="n">
         <v>0.225099</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="n">
+      <c r="B12" s="4" t="n">
         <v>0.140809</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="n">
+      <c r="B13" s="4" t="n">
         <v>0.107298</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="n">
+      <c r="B14" s="4" t="n">
         <v>0.09688</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="n">
+      <c r="B15" s="4" t="n">
         <v>0.079955</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="n">
+      <c r="B16" s="4" t="n">
         <v>0.032781</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="5"/>
+      <c r="B17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="5"/>
+      <c r="B18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="6" t="n">
+      <c r="B21" s="7" t="n">
         <v>0.822979518993796</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="6"/>
+      <c r="B23" s="7"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="6" t="n">
+      <c r="B24" s="7" t="n">
         <v>0.446526</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="6" t="n">
+      <c r="B25" s="7" t="n">
         <v>0.249462</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="6" t="n">
+      <c r="B26" s="7" t="n">
         <v>0.174723</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="6" t="n">
+      <c r="B27" s="7" t="n">
         <v>0.107582</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="6" t="n">
+      <c r="B28" s="7" t="n">
         <v>0.014524</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="6" t="n">
+      <c r="B29" s="7" t="n">
         <v>0.006385</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="6" t="n">
+      <c r="B30" s="7" t="n">
         <v>0.000798</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B32" s="3"/>
+      <c r="B32" s="4"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="3" t="n">
+      <c r="B35" s="4" t="n">
         <v>0.8383</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="3"/>
+      <c r="B36" s="4"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B37" s="3"/>
+      <c r="B37" s="4"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B40" s="3" t="n">
+      <c r="B40" s="4" t="n">
         <v>0.8317</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B44" s="5"/>
+      <c r="B44" s="6"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B47" s="6" t="n">
+      <c r="B47" s="7" t="n">
         <v>0.794085153395088</v>
       </c>
     </row>
@@ -643,312 +654,315 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="3"/>
+      <c r="B2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="3"/>
+      <c r="B3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3" t="n">
+      <c r="B7" s="4" t="n">
         <v>0.354550862581796</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="5"/>
+      <c r="B8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="n">
+      <c r="B10" s="4" t="n">
         <v>0.424503</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="3" t="n">
+      <c r="B11" s="4" t="n">
         <v>0.217831</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="n">
+      <c r="B12" s="4" t="n">
         <v>0.130594</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="3" t="n">
+      <c r="B13" s="4" t="n">
         <v>0.113796</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="3" t="n">
+      <c r="B14" s="4" t="n">
         <v>0.066708</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="3" t="n">
+      <c r="B15" s="4" t="n">
         <v>0.027254</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="3" t="n">
+      <c r="B16" s="4" t="n">
         <v>0.019315</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="5"/>
+      <c r="B17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="5"/>
+      <c r="B18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="6" t="n">
+      <c r="B21" s="7" t="n">
         <v>0.425766975439789</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="6"/>
+      <c r="B23" s="7"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="3" t="n">
+      <c r="B24" s="4" t="n">
         <v>0.626215</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="3" t="n">
+      <c r="B25" s="4" t="n">
         <v>0.192116</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="3" t="n">
+      <c r="B26" s="4" t="n">
         <v>0.123391</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="3" t="n">
+      <c r="B27" s="4" t="n">
         <v>0.050198</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="3" t="n">
+      <c r="B28" s="4" t="n">
         <v>0.005109</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="3" t="n">
+      <c r="B29" s="4" t="n">
         <v>0.0026</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="3" t="n">
+      <c r="B30" s="4" t="n">
         <v>0.000371</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B32" s="3"/>
+      <c r="B32" s="4"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="3" t="n">
+      <c r="B35" s="4" t="n">
         <v>0.4315</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="3"/>
+      <c r="B36" s="4"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B37" s="3"/>
+      <c r="B37" s="4"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B40" s="3" t="n">
+      <c r="B40" s="4" t="n">
         <v>0.3718</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B44" s="5"/>
+      <c r="B44" s="6"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B47" s="6" t="n">
+      <c r="B47" s="7" t="n">
         <v>0.363049205404946</v>
       </c>
     </row>
@@ -968,337 +982,351 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="7" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="8" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="9"/>
+      <c r="B1" s="10"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0"/>
-      <c r="B2" s="10"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0"/>
-      <c r="B3" s="10"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="10"/>
+      <c r="B4" s="11"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="11" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="10" t="n">
-        <v>0.57644259369423</v>
+      <c r="B7" s="11" t="n">
+        <v>0.650293192827399</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0"/>
-      <c r="B8" s="9"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="9"/>
+      <c r="B9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="8" t="n">
+        <v>0.883294</v>
+      </c>
+      <c r="I10" s="0"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8" t="n">
+        <v>0.055726</v>
+      </c>
+      <c r="I11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="8" t="n">
+        <v>0.033004</v>
+      </c>
+      <c r="H12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="8" t="n">
+        <v>0.010788</v>
+      </c>
+      <c r="F13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="10" t="n">
-        <v>0.530166</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
+      <c r="B14" s="8" t="n">
+        <v>0.010688</v>
+      </c>
+      <c r="E14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="10" t="n">
-        <v>0.220887</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="s">
+      <c r="B15" s="8" t="n">
+        <v>0.0065</v>
+      </c>
+      <c r="I15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2"/>
+      <c r="B17" s="10"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="10"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="13" t="n">
+        <v>0.650548143112093</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="13"/>
+      <c r="B22" s="13"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="13"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="10" t="n">
-        <v>0.17522</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="s">
+      <c r="B24" s="14" t="n">
+        <v>0.707396</v>
+      </c>
+      <c r="I24" s="0"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="10" t="n">
-        <v>0.03269</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9" t="s">
+      <c r="B25" s="14" t="n">
+        <v>0.116373</v>
+      </c>
+      <c r="H25" s="0"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="14" t="n">
+        <v>0.070952</v>
+      </c>
+      <c r="I26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="10" t="n">
-        <v>0.019525</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="10" t="n">
-        <v>0.016092</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9" t="s">
+      <c r="B27" s="14" t="n">
+        <v>0.033274</v>
+      </c>
+      <c r="F27" s="0"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="14" t="n">
+        <v>0.029272</v>
+      </c>
+      <c r="E28" s="0"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="10" t="n">
-        <v>0.00542</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0"/>
-      <c r="B17" s="9"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11" t="s">
+      <c r="B29" s="14" t="n">
+        <v>0.024967</v>
+      </c>
+      <c r="F29" s="0"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="14" t="n">
+        <v>0.017766</v>
+      </c>
+      <c r="I30" s="0"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="13"/>
+      <c r="B31" s="13"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="11"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="11" t="n">
+        <v>0.6524</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2"/>
+      <c r="B36" s="11"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="11"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40" s="11" t="n">
+        <v>0.658</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2"/>
+      <c r="B41" s="10"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2"/>
+      <c r="B42" s="10"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B43" s="2"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="9"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12" t="s">
+      <c r="B44" s="10"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B45" s="13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="12" t="s">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B46" s="13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12" t="s">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="12" t="n">
-        <v>0.600747854168437</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="12"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" s="10" t="n">
-        <v>0.619166</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="10" t="n">
-        <v>0.179677</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="10" t="n">
-        <v>0.162222</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="10" t="n">
-        <v>0.019415</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="10" t="n">
-        <v>0.010499</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" s="10" t="n">
-        <v>0.005397</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B30" s="10" t="n">
-        <v>0.003624</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B32" s="10"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B35" s="10" t="n">
-        <v>0.646</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0"/>
-      <c r="B36" s="10"/>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B37" s="10"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B40" s="10" t="n">
-        <v>0.656</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0"/>
-      <c r="B41" s="9"/>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0"/>
-      <c r="B42" s="9"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B43" s="0"/>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B44" s="9"/>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B47" s="12" t="n">
-        <v>0.600747854168437</v>
+      <c r="B47" s="13" t="n">
+        <v>0.6547</v>
       </c>
     </row>
   </sheetData>

</xml_diff>